<commit_message>
changed kane_census_mock.xls to match current format of provided file
</commit_message>
<xml_diff>
--- a/test/mock/kane_census_mock.xlsx
+++ b/test/mock/kane_census_mock.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sds25\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\documents\wprdc\wprdc-etl\test\mock\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -27,61 +27,61 @@
     <t>GH-Male</t>
   </si>
   <si>
-    <t>GH-Female</t>
+    <t xml:space="preserve">GH-Female </t>
   </si>
   <si>
-    <t>GH-White</t>
+    <t xml:space="preserve">GH-White </t>
   </si>
   <si>
-    <t>GH - Black</t>
+    <t xml:space="preserve">GH - Black </t>
   </si>
   <si>
-    <t>GH-Other</t>
+    <t xml:space="preserve">GH-Other </t>
   </si>
   <si>
-    <t>Scott-Male</t>
+    <t xml:space="preserve">Scott-Male </t>
   </si>
   <si>
-    <t>Scott-Female</t>
+    <t xml:space="preserve">Scott-Female </t>
   </si>
   <si>
-    <t>Scott-White</t>
+    <t xml:space="preserve">Scott-White </t>
   </si>
   <si>
-    <t>Scott-Black</t>
+    <t xml:space="preserve">Scott-Black </t>
   </si>
   <si>
-    <t>Scott-Other</t>
+    <t xml:space="preserve">Scott-Other </t>
   </si>
   <si>
-    <t>McK-Male</t>
+    <t xml:space="preserve">McK-Male </t>
   </si>
   <si>
-    <t>McK-Female</t>
+    <t xml:space="preserve">McK-Female </t>
   </si>
   <si>
-    <t>McK-White</t>
+    <t xml:space="preserve">McK-White </t>
   </si>
   <si>
-    <t>McK-Black</t>
+    <t xml:space="preserve">McK-Black </t>
   </si>
   <si>
-    <t>McK-Other</t>
+    <t xml:space="preserve">McK-Other </t>
   </si>
   <si>
-    <t>Ross-Male</t>
+    <t xml:space="preserve">Ross-Male </t>
   </si>
   <si>
-    <t>Ross-Female</t>
+    <t xml:space="preserve">Ross-Female </t>
   </si>
   <si>
-    <t>Ross-White</t>
+    <t xml:space="preserve">Ross-White </t>
   </si>
   <si>
-    <t>Ross-Black</t>
+    <t xml:space="preserve">Ross-Black </t>
   </si>
   <si>
-    <t>Ross-Other</t>
+    <t xml:space="preserve">Ross-Other </t>
   </si>
 </sst>
 </file>
@@ -891,8 +891,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="U1" sqref="U1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>